<commit_message>
added calculations to sheet
</commit_message>
<xml_diff>
--- a/exp10/data/values.xlsx
+++ b/exp10/data/values.xlsx
@@ -16,14 +16,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="18">
   <si>
     <t>Offset L-ruler</t>
   </si>
   <si>
-    <t>130mm</t>
-  </si>
-  <si>
     <t>Heat:</t>
   </si>
   <si>
@@ -43,19 +40,55 @@
   </si>
   <si>
     <t>bigcirc rad [mm]</t>
+  </si>
+  <si>
+    <t>[mm]</t>
+  </si>
+  <si>
+    <t>bigcirc-small</t>
+  </si>
+  <si>
+    <t>L-&gt;small</t>
+  </si>
+  <si>
+    <t>r[mm]</t>
+  </si>
+  <si>
+    <t>B [T]</t>
+  </si>
+  <si>
+    <t>mu_0</t>
+  </si>
+  <si>
+    <t>(4/5)^(1.5)</t>
+  </si>
+  <si>
+    <t>r(theor)</t>
+  </si>
+  <si>
+    <t>e/m</t>
+  </si>
+  <si>
+    <t>%dev</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="1">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -78,8 +111,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="11" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -374,46 +409,98 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A2:E20"/>
+  <dimension ref="A1:M22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A21" sqref="A21"/>
+      <selection activeCell="M8" sqref="M8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <cols>
+    <col min="3" max="3" width="14" customWidth="1"/>
+    <col min="4" max="4" width="16" customWidth="1"/>
+    <col min="5" max="5" width="15" customWidth="1"/>
+    <col min="9" max="11" width="12" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="12.42578125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="2" spans="1:5">
+    <row r="1" spans="1:13">
+      <c r="B1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13">
       <c r="A2" t="s">
         <v>0</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2">
+        <v>130</v>
+      </c>
+      <c r="C2" t="s">
         <v>1</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>2</v>
       </c>
-      <c r="D2" t="s">
+      <c r="H2" t="s">
+        <v>13</v>
+      </c>
+      <c r="I2">
+        <f>1.25663706144*10^(-6)</f>
+        <v>1.25663706144E-6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13">
+      <c r="H3" t="s">
+        <v>14</v>
+      </c>
+      <c r="I3">
+        <f>(4/5)^(1.5)</f>
+        <v>0.71554175279993271</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13">
+      <c r="A7" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="7" spans="1:5">
-      <c r="A7" t="s">
+      <c r="B7" t="s">
         <v>4</v>
       </c>
-      <c r="B7" t="s">
+      <c r="C7" t="s">
         <v>5</v>
       </c>
-      <c r="C7" t="s">
+      <c r="D7" t="s">
+        <v>7</v>
+      </c>
+      <c r="E7" t="s">
         <v>6</v>
       </c>
-      <c r="D7" t="s">
-        <v>8</v>
-      </c>
-      <c r="E7" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5">
+      <c r="F7" t="s">
+        <v>10</v>
+      </c>
+      <c r="G7" t="s">
+        <v>9</v>
+      </c>
+      <c r="H7" t="s">
+        <v>11</v>
+      </c>
+      <c r="I7" t="s">
+        <v>12</v>
+      </c>
+      <c r="J7" t="s">
+        <v>15</v>
+      </c>
+      <c r="K7" t="s">
+        <v>16</v>
+      </c>
+      <c r="L7" t="s">
+        <v>16</v>
+      </c>
+      <c r="M7" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13">
       <c r="A8">
         <v>303.8</v>
       </c>
@@ -429,8 +516,40 @@
       <c r="E8">
         <v>50</v>
       </c>
-    </row>
-    <row r="9" spans="1:5">
+      <c r="F8">
+        <f>$B$2+C8*10+G8</f>
+        <v>630</v>
+      </c>
+      <c r="G8">
+        <f>(E8-C8)*10</f>
+        <v>241.5</v>
+      </c>
+      <c r="H8">
+        <f>(F8*D8/G8)/2</f>
+        <v>28.173913043478262</v>
+      </c>
+      <c r="I8">
+        <f>$I$3*$I$2*124*B8/0.15</f>
+        <v>2.1556252819545192E-3</v>
+      </c>
+      <c r="J8">
+        <f>(3.37212982702*10^(-6)*SQRT(A8)/I8)*1000</f>
+        <v>27.266218011510151</v>
+      </c>
+      <c r="K8">
+        <f>2*A8/((H8/1000)^2*I8^2)</f>
+        <v>164731589303.24161</v>
+      </c>
+      <c r="L8" s="1">
+        <f>1.758820088*10^11</f>
+        <v>175882008800</v>
+      </c>
+      <c r="M8">
+        <f>100-L8/K8*100</f>
+        <v>-6.7688410850164473</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13">
       <c r="A9">
         <v>303.8</v>
       </c>
@@ -446,8 +565,40 @@
       <c r="E9">
         <v>50</v>
       </c>
-    </row>
-    <row r="10" spans="1:5">
+      <c r="F9">
+        <f t="shared" ref="F9:F20" si="0">$B$2+C9*10+G9</f>
+        <v>630</v>
+      </c>
+      <c r="G9">
+        <f t="shared" ref="G9:G20" si="1">(E9-C9)*10</f>
+        <v>235.5</v>
+      </c>
+      <c r="H9">
+        <f t="shared" ref="H9:H20" si="2">(F9*D9/G9)/2</f>
+        <v>28.891719745222929</v>
+      </c>
+      <c r="I9">
+        <f t="shared" ref="I9:I20" si="3">$I$3*$I$2*124*B9/0.15</f>
+        <v>2.1556252819545192E-3</v>
+      </c>
+      <c r="J9">
+        <f t="shared" ref="J9:J20" si="4">(3.37212982702*10^(-6)*SQRT(A9)/I9)*1000</f>
+        <v>27.266218011510151</v>
+      </c>
+      <c r="K9">
+        <f t="shared" ref="K9:K20" si="5">2*A9/((H9/1000)^2*I9^2)</f>
+        <v>156647850960.05563</v>
+      </c>
+      <c r="L9" s="1">
+        <f t="shared" ref="L9:L20" si="6">1.758820088*10^11</f>
+        <v>175882008800</v>
+      </c>
+      <c r="M9">
+        <f t="shared" ref="M9:M20" si="7">100-L9/K9*100</f>
+        <v>-12.278596688089237</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13">
       <c r="A10">
         <v>304</v>
       </c>
@@ -463,8 +614,40 @@
       <c r="E10">
         <v>50</v>
       </c>
-    </row>
-    <row r="11" spans="1:5">
+      <c r="F10">
+        <f t="shared" si="0"/>
+        <v>630</v>
+      </c>
+      <c r="G10">
+        <f t="shared" si="1"/>
+        <v>256</v>
+      </c>
+      <c r="H10">
+        <f t="shared" si="2"/>
+        <v>48.7265625</v>
+      </c>
+      <c r="I10">
+        <f t="shared" si="3"/>
+        <v>1.2562092160355648E-3</v>
+      </c>
+      <c r="J10">
+        <f t="shared" si="4"/>
+        <v>46.8035832020622</v>
+      </c>
+      <c r="K10">
+        <f t="shared" si="5"/>
+        <v>162273678099.25833</v>
+      </c>
+      <c r="L10" s="1">
+        <f t="shared" si="6"/>
+        <v>175882008800</v>
+      </c>
+      <c r="M10">
+        <f t="shared" si="7"/>
+        <v>-8.3860370086748333</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13">
       <c r="A11">
         <v>303.89999999999998</v>
       </c>
@@ -480,8 +663,40 @@
       <c r="E11">
         <v>50</v>
       </c>
-    </row>
-    <row r="12" spans="1:5">
+      <c r="F11">
+        <f t="shared" si="0"/>
+        <v>630</v>
+      </c>
+      <c r="G11">
+        <f t="shared" si="1"/>
+        <v>393.5</v>
+      </c>
+      <c r="H11">
+        <f t="shared" si="2"/>
+        <v>17.29097839898348</v>
+      </c>
+      <c r="I11">
+        <f t="shared" si="3"/>
+        <v>3.6794293605775419E-3</v>
+      </c>
+      <c r="J11">
+        <f t="shared" si="4"/>
+        <v>15.976776766227191</v>
+      </c>
+      <c r="K11">
+        <f t="shared" si="5"/>
+        <v>150162199210.94299</v>
+      </c>
+      <c r="L11" s="1">
+        <f t="shared" si="6"/>
+        <v>175882008800</v>
+      </c>
+      <c r="M11">
+        <f t="shared" si="7"/>
+        <v>-17.128018718563553</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13">
       <c r="A12">
         <v>304</v>
       </c>
@@ -497,8 +712,40 @@
       <c r="E12">
         <v>50</v>
       </c>
-    </row>
-    <row r="13" spans="1:5">
+      <c r="F12">
+        <f t="shared" si="0"/>
+        <v>630</v>
+      </c>
+      <c r="G12">
+        <f t="shared" si="1"/>
+        <v>321</v>
+      </c>
+      <c r="H12">
+        <f t="shared" si="2"/>
+        <v>21.196261682242991</v>
+      </c>
+      <c r="I12">
+        <f t="shared" si="3"/>
+        <v>2.9732762509717507E-3</v>
+      </c>
+      <c r="J12">
+        <f t="shared" si="4"/>
+        <v>19.774513902871281</v>
+      </c>
+      <c r="K12">
+        <f t="shared" si="5"/>
+        <v>153078610093.12473</v>
+      </c>
+      <c r="L12" s="1">
+        <f t="shared" si="6"/>
+        <v>175882008800</v>
+      </c>
+      <c r="M12">
+        <f t="shared" si="7"/>
+        <v>-14.896528452278829</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13">
       <c r="A13">
         <v>151.19999999999999</v>
       </c>
@@ -514,8 +761,40 @@
       <c r="E13">
         <v>50</v>
       </c>
-    </row>
-    <row r="14" spans="1:5">
+      <c r="F13">
+        <f t="shared" si="0"/>
+        <v>630</v>
+      </c>
+      <c r="G13">
+        <f t="shared" si="1"/>
+        <v>265</v>
+      </c>
+      <c r="H13">
+        <f t="shared" si="2"/>
+        <v>47.071698113207546</v>
+      </c>
+      <c r="I13">
+        <f t="shared" si="3"/>
+        <v>9.1428244717381337E-4</v>
+      </c>
+      <c r="J13">
+        <f t="shared" si="4"/>
+        <v>45.352350474245199</v>
+      </c>
+      <c r="K13">
+        <f t="shared" si="5"/>
+        <v>163268082102.93082</v>
+      </c>
+      <c r="L13" s="1">
+        <f t="shared" si="6"/>
+        <v>175882008800</v>
+      </c>
+      <c r="M13">
+        <f t="shared" si="7"/>
+        <v>-7.7258987394222203</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13">
       <c r="A14">
         <v>151.30000000000001</v>
       </c>
@@ -531,8 +810,40 @@
       <c r="E14">
         <v>50</v>
       </c>
-    </row>
-    <row r="15" spans="1:5">
+      <c r="F14">
+        <f t="shared" si="0"/>
+        <v>630</v>
+      </c>
+      <c r="G14">
+        <f t="shared" si="1"/>
+        <v>240</v>
+      </c>
+      <c r="H14">
+        <f t="shared" si="2"/>
+        <v>38.85</v>
+      </c>
+      <c r="I14">
+        <f t="shared" si="3"/>
+        <v>1.1372781659966947E-3</v>
+      </c>
+      <c r="J14">
+        <f t="shared" si="4"/>
+        <v>36.47178753126456</v>
+      </c>
+      <c r="K14">
+        <f t="shared" si="5"/>
+        <v>155007772196.98462</v>
+      </c>
+      <c r="L14" s="1">
+        <f t="shared" si="6"/>
+        <v>175882008800</v>
+      </c>
+      <c r="M14">
+        <f t="shared" si="7"/>
+        <v>-13.466574164093075</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13">
       <c r="A15">
         <v>151.30000000000001</v>
       </c>
@@ -548,8 +859,40 @@
       <c r="E15">
         <v>50</v>
       </c>
-    </row>
-    <row r="16" spans="1:5">
+      <c r="F15">
+        <f t="shared" si="0"/>
+        <v>630</v>
+      </c>
+      <c r="G15">
+        <f t="shared" si="1"/>
+        <v>283</v>
+      </c>
+      <c r="H15">
+        <f t="shared" si="2"/>
+        <v>24.042402826855124</v>
+      </c>
+      <c r="I15">
+        <f t="shared" si="3"/>
+        <v>1.8582976568573442E-3</v>
+      </c>
+      <c r="J15">
+        <f t="shared" si="4"/>
+        <v>22.320733969133912</v>
+      </c>
+      <c r="K15">
+        <f t="shared" si="5"/>
+        <v>151594214236.20239</v>
+      </c>
+      <c r="L15" s="1">
+        <f t="shared" si="6"/>
+        <v>175882008800</v>
+      </c>
+      <c r="M15">
+        <f t="shared" si="7"/>
+        <v>-16.021584125865274</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13">
       <c r="A16">
         <v>151.30000000000001</v>
       </c>
@@ -565,8 +908,40 @@
       <c r="E16">
         <v>50</v>
       </c>
-    </row>
-    <row r="17" spans="1:5">
+      <c r="F16">
+        <f t="shared" si="0"/>
+        <v>630</v>
+      </c>
+      <c r="G16">
+        <f t="shared" si="1"/>
+        <v>441.5</v>
+      </c>
+      <c r="H16">
+        <f t="shared" si="2"/>
+        <v>15.411098527746319</v>
+      </c>
+      <c r="I16">
+        <f t="shared" si="3"/>
+        <v>2.8915111540700278E-3</v>
+      </c>
+      <c r="J16">
+        <f t="shared" si="4"/>
+        <v>14.344944710240302</v>
+      </c>
+      <c r="K16">
+        <f t="shared" si="5"/>
+        <v>152388426855.44595</v>
+      </c>
+      <c r="L16" s="1">
+        <f t="shared" si="6"/>
+        <v>175882008800</v>
+      </c>
+      <c r="M16">
+        <f t="shared" si="7"/>
+        <v>-15.416906932729077</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13">
       <c r="A17">
         <v>229.9</v>
       </c>
@@ -582,8 +957,40 @@
       <c r="E17">
         <v>50</v>
       </c>
-    </row>
-    <row r="18" spans="1:5">
+      <c r="F17">
+        <f t="shared" si="0"/>
+        <v>630</v>
+      </c>
+      <c r="G17">
+        <f t="shared" si="1"/>
+        <v>257</v>
+      </c>
+      <c r="H17">
+        <f t="shared" si="2"/>
+        <v>48.536964980544745</v>
+      </c>
+      <c r="I17">
+        <f t="shared" si="3"/>
+        <v>1.1075454034869773E-3</v>
+      </c>
+      <c r="J17">
+        <f t="shared" si="4"/>
+        <v>46.164935510948162</v>
+      </c>
+      <c r="K17">
+        <f t="shared" si="5"/>
+        <v>159111165176.83621</v>
+      </c>
+      <c r="L17" s="1">
+        <f t="shared" si="6"/>
+        <v>175882008800</v>
+      </c>
+      <c r="M17">
+        <f t="shared" si="7"/>
+        <v>-10.540331097773475</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13">
       <c r="A18">
         <v>229.9</v>
       </c>
@@ -599,8 +1006,40 @@
       <c r="E18">
         <v>50</v>
       </c>
-    </row>
-    <row r="19" spans="1:5">
+      <c r="F18">
+        <f t="shared" si="0"/>
+        <v>630</v>
+      </c>
+      <c r="G18">
+        <f t="shared" si="1"/>
+        <v>265</v>
+      </c>
+      <c r="H18">
+        <f t="shared" si="2"/>
+        <v>35.18490566037736</v>
+      </c>
+      <c r="I18">
+        <f t="shared" si="3"/>
+        <v>1.4866381254858754E-3</v>
+      </c>
+      <c r="J18">
+        <f t="shared" si="4"/>
+        <v>34.392876955656384</v>
+      </c>
+      <c r="K18">
+        <f t="shared" si="5"/>
+        <v>168052761193.32257</v>
+      </c>
+      <c r="L18" s="1">
+        <f t="shared" si="6"/>
+        <v>175882008800</v>
+      </c>
+      <c r="M18">
+        <f t="shared" si="7"/>
+        <v>-4.6588033133659223</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13">
       <c r="A19">
         <v>229.9</v>
       </c>
@@ -616,8 +1055,40 @@
       <c r="E19">
         <v>50</v>
       </c>
-    </row>
-    <row r="20" spans="1:5">
+      <c r="F19">
+        <f t="shared" si="0"/>
+        <v>630</v>
+      </c>
+      <c r="G19">
+        <f t="shared" si="1"/>
+        <v>266.5</v>
+      </c>
+      <c r="H19">
+        <f t="shared" si="2"/>
+        <v>25.530956848030019</v>
+      </c>
+      <c r="I19">
+        <f t="shared" si="3"/>
+        <v>2.0812933756802253E-3</v>
+      </c>
+      <c r="J19">
+        <f t="shared" si="4"/>
+        <v>24.566340682611706</v>
+      </c>
+      <c r="K19">
+        <f t="shared" si="5"/>
+        <v>162842656994.42926</v>
+      </c>
+      <c r="L19" s="1">
+        <f t="shared" si="6"/>
+        <v>175882008800</v>
+      </c>
+      <c r="M19">
+        <f t="shared" si="7"/>
+        <v>-8.0073317681231373</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13">
       <c r="A20">
         <v>229.9</v>
       </c>
@@ -633,10 +1104,52 @@
       <c r="E20">
         <v>50</v>
       </c>
+      <c r="F20">
+        <f t="shared" si="0"/>
+        <v>630</v>
+      </c>
+      <c r="G20">
+        <f t="shared" si="1"/>
+        <v>370</v>
+      </c>
+      <c r="H20">
+        <f t="shared" si="2"/>
+        <v>18.389189189189189</v>
+      </c>
+      <c r="I20">
+        <f t="shared" si="3"/>
+        <v>2.9732762509717507E-3</v>
+      </c>
+      <c r="J20">
+        <f t="shared" si="4"/>
+        <v>17.196438477828192</v>
+      </c>
+      <c r="K20">
+        <f t="shared" si="5"/>
+        <v>153806001272.0423</v>
+      </c>
+      <c r="L20" s="1">
+        <f t="shared" si="6"/>
+        <v>175882008800</v>
+      </c>
+      <c r="M20">
+        <f t="shared" si="7"/>
+        <v>-14.353150946893848</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13">
+      <c r="K22">
+        <f>AVERAGE(K8:K20)</f>
+        <v>157920385207.29364</v>
+      </c>
+      <c r="L22" s="2">
+        <f>STDEV(K8:K20)/SQRT(COUNT(K8:K20))</f>
+        <v>1608350272.8531902</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="0" orientation="portrait" horizontalDpi="0" verticalDpi="0" copies="0"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
asdfsad 	modified:   exp10/data/values.xlsx 	modified:   exp10/report/report10.tex
</commit_message>
<xml_diff>
--- a/exp10/data/values.xlsx
+++ b/exp10/data/values.xlsx
@@ -92,15 +92,13 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="8">
+  <numFmts count="6">
     <numFmt formatCode="GENERAL" numFmtId="164"/>
-    <numFmt formatCode="GENERAL" numFmtId="165"/>
-    <numFmt formatCode="0.000" numFmtId="166"/>
-    <numFmt formatCode="0.000" numFmtId="167"/>
-    <numFmt formatCode="0.###" numFmtId="168"/>
-    <numFmt formatCode="0.00" numFmtId="169"/>
-    <numFmt formatCode="0.0000" numFmtId="170"/>
-    <numFmt formatCode="0.0000" numFmtId="171"/>
+    <numFmt formatCode="0.000" numFmtId="165"/>
+    <numFmt formatCode="0.###" numFmtId="166"/>
+    <numFmt formatCode="0.000E+000" numFmtId="167"/>
+    <numFmt formatCode="0.00" numFmtId="168"/>
+    <numFmt formatCode="0.0000" numFmtId="169"/>
   </numFmts>
   <fonts count="4">
     <font>
@@ -174,16 +172,20 @@
     <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="42"/>
     <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="9"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="8">
     <xf applyAlignment="false" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0">
       <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
       <protection hidden="false" locked="true"/>
     </xf>
-    <xf applyAlignment="false" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="165" xfId="0">
+    <xf applyAlignment="false" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0">
       <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
       <protection hidden="false" locked="true"/>
     </xf>
     <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="2" fontId="0" numFmtId="164" xfId="0">
+      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
+    <xf applyAlignment="false" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="165" xfId="0">
       <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
       <protection hidden="false" locked="true"/>
     </xf>
@@ -200,14 +202,6 @@
       <protection hidden="false" locked="true"/>
     </xf>
     <xf applyAlignment="false" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="169" xfId="0">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf applyAlignment="false" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="170" xfId="0">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf applyAlignment="false" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="171" xfId="0">
       <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
       <protection hidden="false" locked="true"/>
     </xf>
@@ -288,10 +282,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:O22"/>
+  <dimension ref="A1:Q22"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="K4" activeCellId="0" pane="topLeft" sqref="K4"/>
+    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="F1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
+      <selection activeCell="Q8" activeCellId="0" pane="topLeft" sqref="Q8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -301,6 +295,7 @@
     <col collapsed="false" hidden="false" max="4" min="4" style="0" width="10.834008097166"/>
     <col collapsed="false" hidden="false" max="5" min="5" style="0" width="8.1336032388664"/>
     <col collapsed="false" hidden="false" max="6" min="6" style="0" width="9.1417004048583"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="8.5748987854251"/>
     <col collapsed="false" hidden="false" max="8" min="8" style="0" width="11.1255060728745"/>
     <col collapsed="false" hidden="false" max="9" min="9" style="0" width="11.9959514170041"/>
     <col collapsed="false" hidden="false" max="10" min="10" style="0" width="7.93927125506073"/>
@@ -443,7 +438,7 @@
         <f aca="false">$D$4*$D$3*124*B8/0.15</f>
         <v>0.00215562528195452</v>
       </c>
-      <c r="J8" s="4" t="n">
+      <c r="J8" s="3" t="n">
         <f aca="false">SQRT((D8/1000)^2*$K$4^2/(E8/100-C8/100)^4+(D8/1000)^2*$K$5^2/(E8/100-C8/100)^4)*1000</f>
         <v>1.12639404905024</v>
       </c>
@@ -451,15 +446,15 @@
         <f aca="false">(3.37212982702*10^(-6)*SQRT(A8)/I8)*1000</f>
         <v>27.2662180115101</v>
       </c>
-      <c r="L8" s="5" t="n">
+      <c r="L8" s="4" t="n">
         <f aca="false">2*A8/((H8/1000)^2*I8^2)/(10^11)</f>
         <v>1.64731589303242</v>
       </c>
-      <c r="M8" s="4" t="n">
+      <c r="M8" s="3" t="n">
         <f aca="false">4*(J8/1000)*(A8)/(($D$4*$D$3*124*B8/0.15)^2*(H8/1000)^3)/(10^11)</f>
         <v>0.131719496397546</v>
       </c>
-      <c r="N8" s="0" t="n">
+      <c r="N8" s="5" t="n">
         <f aca="false">1.758820088*10^11</f>
         <v>175882008800</v>
       </c>
@@ -467,6 +462,10 @@
         <f aca="false">100-N8/L8/10^11*100</f>
         <v>-6.7688410850165</v>
       </c>
+      <c r="Q8" s="0" t="n">
+        <f aca="false">100-100*(L22*10^11)/N8</f>
+        <v>10.2123143323494</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="9">
       <c r="A9" s="0" t="n">
@@ -500,7 +499,7 @@
         <f aca="false">$D$4*$D$3*124*B9/0.15</f>
         <v>0.00215562528195452</v>
       </c>
-      <c r="J9" s="4" t="n">
+      <c r="J9" s="3" t="n">
         <f aca="false">SQRT((D9/1000)^2*$K$4^2/(E9/100-C9/100)^4+(D9/1000)^2*$K$5^2/(E9/100-C9/100)^4)*1000</f>
         <v>1.18452108180581</v>
       </c>
@@ -508,15 +507,15 @@
         <f aca="false">(3.37212982702*10^(-6)*SQRT(A9)/I9)*1000</f>
         <v>27.2662180115101</v>
       </c>
-      <c r="L9" s="5" t="n">
+      <c r="L9" s="4" t="n">
         <f aca="false">2*A9/((H9/1000)^2*I9^2)/(10^11)</f>
         <v>1.56647850960056</v>
       </c>
-      <c r="M9" s="4" t="n">
+      <c r="M9" s="3" t="n">
         <f aca="false">4*(J9/1000)*(A9)/(($D$4*$D$3*124*B9/0.15)^2*(H9/1000)^3)/(10^11)</f>
         <v>0.128446962325557</v>
       </c>
-      <c r="N9" s="0" t="n">
+      <c r="N9" s="5" t="n">
         <f aca="false">1.758820088*10^11</f>
         <v>175882008800</v>
       </c>
@@ -557,7 +556,7 @@
         <f aca="false">$D$4*$D$3*124*B10/0.15</f>
         <v>0.00125620921603557</v>
       </c>
-      <c r="J10" s="4" t="n">
+      <c r="J10" s="3" t="n">
         <f aca="false">SQRT((D10/1000)^2*$K$4^2/(E10/100-C10/100)^4+(D10/1000)^2*$K$5^2/(E10/100-C10/100)^4)*1000</f>
         <v>1.83774868926856</v>
       </c>
@@ -565,15 +564,15 @@
         <f aca="false">(3.37212982702*10^(-6)*SQRT(A10)/I10)*1000</f>
         <v>46.8035832020622</v>
       </c>
-      <c r="L10" s="5" t="n">
+      <c r="L10" s="4" t="n">
         <f aca="false">2*A10/((H10/1000)^2*I10^2)/(10^11)</f>
         <v>1.62273678099258</v>
       </c>
-      <c r="M10" s="4" t="n">
+      <c r="M10" s="3" t="n">
         <f aca="false">4*(J10/1000)*(A10)/(($D$4*$D$3*124*B10/0.15)^2*(H10/1000)^3)/(10^11)</f>
         <v>0.122404792757421</v>
       </c>
-      <c r="N10" s="0" t="n">
+      <c r="N10" s="5" t="n">
         <f aca="false">1.758820088*10^11</f>
         <v>175882008800</v>
       </c>
@@ -614,7 +613,7 @@
         <f aca="false">$D$4*$D$3*124*B11/0.15</f>
         <v>0.00367942936057754</v>
       </c>
-      <c r="J11" s="4" t="n">
+      <c r="J11" s="3" t="n">
         <f aca="false">SQRT((D11/1000)^2*$K$4^2/(E11/100-C11/100)^4+(D11/1000)^2*$K$5^2/(E11/100-C11/100)^4)*1000</f>
         <v>0.424262985891903</v>
       </c>
@@ -622,15 +621,15 @@
         <f aca="false">(3.37212982702*10^(-6)*SQRT(A11)/I11)*1000</f>
         <v>15.9767767662272</v>
       </c>
-      <c r="L11" s="5" t="n">
+      <c r="L11" s="4" t="n">
         <f aca="false">2*A11/((H11/1000)^2*I11^2)/(10^11)</f>
         <v>1.50162199210943</v>
       </c>
-      <c r="M11" s="4" t="n">
+      <c r="M11" s="3" t="n">
         <f aca="false">4*(J11/1000)*(A11)/(($D$4*$D$3*124*B11/0.15)^2*(H11/1000)^3)/(10^11)</f>
         <v>0.0736895987436718</v>
       </c>
-      <c r="N11" s="0" t="n">
+      <c r="N11" s="5" t="n">
         <f aca="false">1.758820088*10^11</f>
         <v>175882008800</v>
       </c>
@@ -671,7 +670,7 @@
         <f aca="false">$D$4*$D$3*124*B12/0.15</f>
         <v>0.00297327625097175</v>
       </c>
-      <c r="J12" s="4" t="n">
+      <c r="J12" s="3" t="n">
         <f aca="false">SQRT((D12/1000)^2*$K$4^2/(E12/100-C12/100)^4+(D12/1000)^2*$K$5^2/(E12/100-C12/100)^4)*1000</f>
         <v>0.637550444262192</v>
       </c>
@@ -679,15 +678,15 @@
         <f aca="false">(3.37212982702*10^(-6)*SQRT(A12)/I12)*1000</f>
         <v>19.7745139028713</v>
       </c>
-      <c r="L12" s="5" t="n">
+      <c r="L12" s="4" t="n">
         <f aca="false">2*A12/((H12/1000)^2*I12^2)/(10^11)</f>
         <v>1.53078610093125</v>
       </c>
-      <c r="M12" s="4" t="n">
+      <c r="M12" s="3" t="n">
         <f aca="false">4*(J12/1000)*(A12)/(($D$4*$D$3*124*B12/0.15)^2*(H12/1000)^3)/(10^11)</f>
         <v>0.0920873098615028</v>
       </c>
-      <c r="N12" s="0" t="n">
+      <c r="N12" s="5" t="n">
         <f aca="false">1.758820088*10^11</f>
         <v>175882008800</v>
       </c>
@@ -728,7 +727,7 @@
         <f aca="false">$D$4*$D$3*124*B13/0.15</f>
         <v>0.000914282447173813</v>
       </c>
-      <c r="J13" s="4" t="n">
+      <c r="J13" s="3" t="n">
         <f aca="false">SQRT((D13/1000)^2*$K$4^2/(E13/100-C13/100)^4+(D13/1000)^2*$K$5^2/(E13/100-C13/100)^4)*1000</f>
         <v>1.71504020078183</v>
       </c>
@@ -736,15 +735,15 @@
         <f aca="false">(3.37212982702*10^(-6)*SQRT(A13)/I13)*1000</f>
         <v>45.3523504742452</v>
       </c>
-      <c r="L13" s="5" t="n">
+      <c r="L13" s="4" t="n">
         <f aca="false">2*A13/((H13/1000)^2*I13^2)/(10^11)</f>
         <v>1.63268082102931</v>
       </c>
-      <c r="M13" s="4" t="n">
+      <c r="M13" s="3" t="n">
         <f aca="false">4*(J13/1000)*(A13)/(($D$4*$D$3*124*B13/0.15)^2*(H13/1000)^3)/(10^11)</f>
         <v>0.118972263816635</v>
       </c>
-      <c r="N13" s="0" t="n">
+      <c r="N13" s="5" t="n">
         <f aca="false">1.758820088*10^11</f>
         <v>175882008800</v>
       </c>
@@ -785,7 +784,7 @@
         <f aca="false">$D$4*$D$3*124*B14/0.15</f>
         <v>0.00113727816599669</v>
       </c>
-      <c r="J14" s="4" t="n">
+      <c r="J14" s="3" t="n">
         <f aca="false">SQRT((D14/1000)^2*$K$4^2/(E14/100-C14/100)^4+(D14/1000)^2*$K$5^2/(E14/100-C14/100)^4)*1000</f>
         <v>1.56293203903495</v>
       </c>
@@ -793,15 +792,15 @@
         <f aca="false">(3.37212982702*10^(-6)*SQRT(A14)/I14)*1000</f>
         <v>36.4717875312646</v>
       </c>
-      <c r="L14" s="5" t="n">
+      <c r="L14" s="4" t="n">
         <f aca="false">2*A14/((H14/1000)^2*I14^2)/(10^11)</f>
         <v>1.55007772196985</v>
       </c>
-      <c r="M14" s="4" t="n">
+      <c r="M14" s="3" t="n">
         <f aca="false">4*(J14/1000)*(A14)/(($D$4*$D$3*124*B14/0.15)^2*(H14/1000)^3)/(10^11)</f>
         <v>0.124718977331325</v>
       </c>
-      <c r="N14" s="0" t="n">
+      <c r="N14" s="5" t="n">
         <f aca="false">1.758820088*10^11</f>
         <v>175882008800</v>
       </c>
@@ -842,7 +841,7 @@
         <f aca="false">$D$4*$D$3*124*B15/0.15</f>
         <v>0.00185829765685734</v>
       </c>
-      <c r="J15" s="4" t="n">
+      <c r="J15" s="3" t="n">
         <f aca="false">SQRT((D15/1000)^2*$K$4^2/(E15/100-C15/100)^4+(D15/1000)^2*$K$5^2/(E15/100-C15/100)^4)*1000</f>
         <v>0.82026040189315</v>
       </c>
@@ -850,15 +849,15 @@
         <f aca="false">(3.37212982702*10^(-6)*SQRT(A15)/I15)*1000</f>
         <v>22.3207339691339</v>
       </c>
-      <c r="L15" s="5" t="n">
+      <c r="L15" s="4" t="n">
         <f aca="false">2*A15/((H15/1000)^2*I15^2)/(10^11)</f>
         <v>1.51594214236202</v>
       </c>
-      <c r="M15" s="4" t="n">
+      <c r="M15" s="3" t="n">
         <f aca="false">4*(J15/1000)*(A15)/(($D$4*$D$3*124*B15/0.15)^2*(H15/1000)^3)/(10^11)</f>
         <v>0.103439520575015</v>
       </c>
-      <c r="N15" s="0" t="n">
+      <c r="N15" s="5" t="n">
         <f aca="false">1.758820088*10^11</f>
         <v>175882008800</v>
       </c>
@@ -899,7 +898,7 @@
         <f aca="false">$D$4*$D$3*124*B16/0.15</f>
         <v>0.00289151115407003</v>
       </c>
-      <c r="J16" s="4" t="n">
+      <c r="J16" s="3" t="n">
         <f aca="false">SQRT((D16/1000)^2*$K$4^2/(E16/100-C16/100)^4+(D16/1000)^2*$K$5^2/(E16/100-C16/100)^4)*1000</f>
         <v>0.337025841468691</v>
       </c>
@@ -907,15 +906,15 @@
         <f aca="false">(3.37212982702*10^(-6)*SQRT(A16)/I16)*1000</f>
         <v>14.3449447102403</v>
       </c>
-      <c r="L16" s="5" t="n">
+      <c r="L16" s="4" t="n">
         <f aca="false">2*A16/((H16/1000)^2*I16^2)/(10^11)</f>
         <v>1.52388426855446</v>
       </c>
-      <c r="M16" s="4" t="n">
+      <c r="M16" s="3" t="n">
         <f aca="false">4*(J16/1000)*(A16)/(($D$4*$D$3*124*B16/0.15)^2*(H16/1000)^3)/(10^11)</f>
         <v>0.0666517545113084</v>
       </c>
-      <c r="N16" s="0" t="n">
+      <c r="N16" s="5" t="n">
         <f aca="false">1.758820088*10^11</f>
         <v>175882008800</v>
       </c>
@@ -956,7 +955,7 @@
         <f aca="false">$D$4*$D$3*124*B17/0.15</f>
         <v>0.00110754540348698</v>
       </c>
-      <c r="J17" s="4" t="n">
+      <c r="J17" s="3" t="n">
         <f aca="false">SQRT((D17/1000)^2*$K$4^2/(E17/100-C17/100)^4+(D17/1000)^2*$K$5^2/(E17/100-C17/100)^4)*1000</f>
         <v>1.82347496706845</v>
       </c>
@@ -964,15 +963,15 @@
         <f aca="false">(3.37212982702*10^(-6)*SQRT(A17)/I17)*1000</f>
         <v>46.1649355109482</v>
       </c>
-      <c r="L17" s="5" t="n">
+      <c r="L17" s="4" t="n">
         <f aca="false">2*A17/((H17/1000)^2*I17^2)/(10^11)</f>
         <v>1.59111165176836</v>
       </c>
-      <c r="M17" s="4" t="n">
+      <c r="M17" s="3" t="n">
         <f aca="false">4*(J17/1000)*(A17)/(($D$4*$D$3*124*B17/0.15)^2*(H17/1000)^3)/(10^11)</f>
         <v>0.119552273941047</v>
       </c>
-      <c r="N17" s="0" t="n">
+      <c r="N17" s="5" t="n">
         <f aca="false">1.758820088*10^11</f>
         <v>175882008800</v>
       </c>
@@ -1013,7 +1012,7 @@
         <f aca="false">$D$4*$D$3*124*B18/0.15</f>
         <v>0.00148663812548588</v>
       </c>
-      <c r="J18" s="4" t="n">
+      <c r="J18" s="3" t="n">
         <f aca="false">SQRT((D18/1000)^2*$K$4^2/(E18/100-C18/100)^4+(D18/1000)^2*$K$5^2/(E18/100-C18/100)^4)*1000</f>
         <v>1.28194924098844</v>
       </c>
@@ -1021,15 +1020,15 @@
         <f aca="false">(3.37212982702*10^(-6)*SQRT(A18)/I18)*1000</f>
         <v>34.3928769556564</v>
       </c>
-      <c r="L18" s="5" t="n">
+      <c r="L18" s="4" t="n">
         <f aca="false">2*A18/((H18/1000)^2*I18^2)/(10^11)</f>
         <v>1.68052761193322</v>
       </c>
-      <c r="M18" s="4" t="n">
+      <c r="M18" s="3" t="n">
         <f aca="false">4*(J18/1000)*(A18)/(($D$4*$D$3*124*B18/0.15)^2*(H18/1000)^3)/(10^11)</f>
         <v>0.122458824666055</v>
       </c>
-      <c r="N18" s="0" t="n">
+      <c r="N18" s="5" t="n">
         <f aca="false">1.758820088*10^11</f>
         <v>175882008800</v>
       </c>
@@ -1070,7 +1069,7 @@
         <f aca="false">$D$4*$D$3*124*B19/0.15</f>
         <v>0.00208129337568023</v>
       </c>
-      <c r="J19" s="4" t="n">
+      <c r="J19" s="3" t="n">
         <f aca="false">SQRT((D19/1000)^2*$K$4^2/(E19/100-C19/100)^4+(D19/1000)^2*$K$5^2/(E19/100-C19/100)^4)*1000</f>
         <v>0.924975417242069</v>
       </c>
@@ -1078,15 +1077,15 @@
         <f aca="false">(3.37212982702*10^(-6)*SQRT(A19)/I19)*1000</f>
         <v>24.5663406826117</v>
       </c>
-      <c r="L19" s="5" t="n">
+      <c r="L19" s="4" t="n">
         <f aca="false">2*A19/((H19/1000)^2*I19^2)/(10^11)</f>
         <v>1.62842656994429</v>
       </c>
-      <c r="M19" s="4" t="n">
+      <c r="M19" s="3" t="n">
         <f aca="false">4*(J19/1000)*(A19)/(($D$4*$D$3*124*B19/0.15)^2*(H19/1000)^3)/(10^11)</f>
         <v>0.117994366991264</v>
       </c>
-      <c r="N19" s="0" t="n">
+      <c r="N19" s="5" t="n">
         <f aca="false">1.758820088*10^11</f>
         <v>175882008800</v>
       </c>
@@ -1127,7 +1126,7 @@
         <f aca="false">$D$4*$D$3*124*B20/0.15</f>
         <v>0.00297327625097175</v>
       </c>
-      <c r="J20" s="4" t="n">
+      <c r="J20" s="3" t="n">
         <f aca="false">SQRT((D20/1000)^2*$K$4^2/(E20/100-C20/100)^4+(D20/1000)^2*$K$5^2/(E20/100-C20/100)^4)*1000</f>
         <v>0.479867314296717</v>
       </c>
@@ -1135,15 +1134,15 @@
         <f aca="false">(3.37212982702*10^(-6)*SQRT(A20)/I20)*1000</f>
         <v>17.1964384778282</v>
       </c>
-      <c r="L20" s="5" t="n">
+      <c r="L20" s="4" t="n">
         <f aca="false">2*A20/((H20/1000)^2*I20^2)/(10^11)</f>
         <v>1.53806001272042</v>
       </c>
-      <c r="M20" s="4" t="n">
+      <c r="M20" s="3" t="n">
         <f aca="false">4*(J20/1000)*(A20)/(($D$4*$D$3*124*B20/0.15)^2*(H20/1000)^3)/(10^11)</f>
         <v>0.080271590001937</v>
       </c>
-      <c r="N20" s="0" t="n">
+      <c r="N20" s="5" t="n">
         <f aca="false">1.758820088*10^11</f>
         <v>175882008800</v>
       </c>
@@ -1153,17 +1152,15 @@
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="22">
-      <c r="L22" s="5" t="inlineStr">
+      <c r="L22" s="4" t="n">
         <f aca="false">AVERAGE(L8:L20)</f>
-        <is>
-          <t/>
-        </is>
+        <v>1.57920385207294</v>
       </c>
       <c r="M22" s="7" t="n">
         <f aca="false">STDEV(L8:L20)/SQRT(COUNT(L8:L20))</f>
         <v>0.0160835027285313</v>
       </c>
-      <c r="O22" s="8" t="n">
+      <c r="O22" s="7" t="n">
         <f aca="false">M22/L22*100</f>
         <v>1.01845640177608</v>
       </c>

</xml_diff>